<commit_message>
changed folder to 'for_cwms_watershed' to make more obvious.  Moved the siteIDs in ESP_Download to the config.xlsx.  Added script to load R and Java locations.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="14400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="14400" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="3" r:id="rId1"/>
     <sheet name="plot_config" sheetId="1" r:id="rId2"/>
     <sheet name="current_data_tbl" sheetId="4" r:id="rId3"/>
     <sheet name="fcst_tbl" sheetId="5" r:id="rId4"/>
+    <sheet name="download_sites" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Author:</t>
   </si>
@@ -192,6 +193,54 @@
   </si>
   <si>
     <t>plot_config tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IHDW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMNW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOPW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGSW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGDW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPDI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRII </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWRI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORFI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANAW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRYO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHBI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMNO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCDI </t>
+  </si>
+  <si>
+    <t>BRNI</t>
+  </si>
+  <si>
+    <t>nwrfc_site_ids</t>
   </si>
 </sst>
 </file>
@@ -418,6 +467,576 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>182563</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Title 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noGrp="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2381250" y="0"/>
+          <a:ext cx="10515600" cy="1325563"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" rtlCol="0" anchor="ctr">
+          <a:normAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:buNone/>
+            <a:defRPr sz="4400" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Finding NWRFC IDs</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>98323</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>84124</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Content Placeholder 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noGrp="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1543050" y="1447786"/>
+          <a:ext cx="3755923" cy="4351338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" rtlCol="0">
+          <a:normAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="228600" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="1000"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="2800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="685800" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="2400" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="1143000" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="2000" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1600200" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="2057400" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2514600" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2971800" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3429000" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3886200" indent="-228600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="500"/>
+            </a:spcBef>
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Navigate to NWRFC site: https://www.nwrfc.noaa.gov/rfc/</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Click on a specific location</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>NWRFC ID is in parentheses next to full site name (only first four characters are needed for R script)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Example config.xlsx ‘download_sites’ tab:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>340942</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>182563</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>435429</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>75746</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="16201" t="22470" r="4865" b="7502"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5541592" y="1325563"/>
+          <a:ext cx="8019287" cy="4274683"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>216309</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>88490</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121572</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11512959" y="2161765"/>
+          <a:ext cx="481781" cy="245807"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>98323</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>186813</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>143695</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5298973" y="2407574"/>
+          <a:ext cx="6184490" cy="403121"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368811</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28731</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>98323</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>68667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="-5349" t="-1075" r="59707" b="1075"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3740661" y="3457731"/>
+          <a:ext cx="1558312" cy="2516436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1381,7 +2000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -1566,9 +2185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1609,4 +2226,876 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working in computFcstVols function in analysis script. Need to compute inflow volumes to end date of each forecast
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -37,15 +37,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>//DWORSHAK-POOL/ELEV//6HOUR/----E0/</t>
-  </si>
-  <si>
-    <t>//DWORSHAK_OUT/FLOW//6HOUR/----E0/</t>
-  </si>
-  <si>
-    <t>//DWORSHAK_IN/FLOW//6HOUR/----E0/</t>
   </si>
   <si>
     <t>sqlite_tblname</t>
@@ -102,12 +93,6 @@
     <t>CWMS ESP Data Viewer Configuration</t>
   </si>
   <si>
-    <t>//LOWER GRANITE-POOL/ELEV//6HOUR/----E0/</t>
-  </si>
-  <si>
-    <t>//LOWER GRANITE_OUT/FLOW//6HOUR/----E0/</t>
-  </si>
-  <si>
     <t>(Optional) Datum shift (e.g., NAVD88 minus NGVD29) to be applied.  If blank, will be interpretted as zero</t>
   </si>
   <si>
@@ -133,9 +118,6 @@
   </si>
   <si>
     <t>current_data_tbl tab</t>
-  </si>
-  <si>
-    <t>//BROWNLEE_IN/FLOW//6HOUR/----E0/</t>
   </si>
   <si>
     <t>Dworshak Elevation&lt;br&gt;(ft, NGVD29)</t>
@@ -237,12 +219,6 @@
     <t>nwrfc_site_ids</t>
   </si>
   <si>
-    <t>Dworshak Coordinated Fcst: %.1f Maf</t>
-  </si>
-  <si>
-    <t>Brownlee NWD Fcst: %.1f Maf</t>
-  </si>
-  <si>
     <t>download_sites</t>
   </si>
   <si>
@@ -253,6 +229,30 @@
   </si>
   <si>
     <t>Example CWMS ESP Viewer Interface and Configuration Information:</t>
+  </si>
+  <si>
+    <t>//DWORSHAK-POOL/ELEV//6HOUR/------------E0/</t>
+  </si>
+  <si>
+    <t>//DWORSHAK_OUT/FLOW//6HOUR/------------E0/</t>
+  </si>
+  <si>
+    <t>//DWORSHAK_IN/FLOW//6HOUR/------------E0/</t>
+  </si>
+  <si>
+    <t>//LOWER GRANITE-POOL/ELEV//6HOUR/------------E0/</t>
+  </si>
+  <si>
+    <t>//LOWER GRANITE_OUT/FLOW//6HOUR/------------E0/</t>
+  </si>
+  <si>
+    <t>//BROWNLEE_IN/FLOW//6HOUR/------------E0/</t>
+  </si>
+  <si>
+    <t>Dworshak Coordinated Fcst: %.1f Maf [%s]</t>
+  </si>
+  <si>
+    <t>Brownlee NWD Fcst: %.1f Maf [%s]</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1310,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1320,8 +1320,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8715375" y="523874"/>
-          <a:ext cx="2381250" cy="1228725"/>
+          <a:off x="8714254" y="523874"/>
+          <a:ext cx="2363321" cy="1638861"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2353,7 +2353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2369,7 +2369,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="4" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -2428,25 +2428,25 @@
     </row>
     <row r="7" spans="1:10" ht="62.25" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="9">
         <v>3.3</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>2</v>
@@ -2454,58 +2454,58 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="9">
         <v>3.4</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="9">
         <v>3.2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9">
         <v>3.3</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12" s="9">
         <v>3.4</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2514,12 +2514,12 @@
     </row>
     <row r="15" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E15" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E16" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>2</v>
@@ -2527,26 +2527,26 @@
     </row>
     <row r="17" spans="5:6" ht="30" x14ac:dyDescent="0.25">
       <c r="E17" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="5:6" ht="45" x14ac:dyDescent="0.25">
       <c r="E18" s="15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
@@ -2557,13 +2557,13 @@
     </row>
     <row r="22" spans="5:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E22" s="14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>2</v>
@@ -2571,44 +2571,44 @@
     </row>
     <row r="24" spans="5:6" ht="30" x14ac:dyDescent="0.25">
       <c r="E24" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="F26" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="5:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E31" s="14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>2</v>
@@ -2616,10 +2616,10 @@
     </row>
     <row r="33" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="E33" s="12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
     </row>
     <row r="38" spans="3:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C38" s="11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2655,13 +2655,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="21" bestFit="1" customWidth="1"/>
@@ -2672,19 +2672,19 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2704,10 +2704,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D2" s="25">
         <v>-3.3</v>
@@ -2731,10 +2731,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25">
@@ -2758,10 +2758,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25">
@@ -2785,10 +2785,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D5" s="25">
         <v>-3.4</v>
@@ -2812,10 +2812,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25">
@@ -2839,10 +2839,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="25">
@@ -3923,7 +3923,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3935,13 +3935,13 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3966,13 +3966,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="25">
         <v>1000</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3997,13 +3997,13 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="25">
         <v>1000</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5513,7 +5513,7 @@
   <dimension ref="A1:AC83"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5526,16 +5526,16 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5565,10 +5565,10 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="C2" s="24">
         <v>43556</v>
@@ -8114,7 +8114,6 @@
       <c r="AC83" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="A2:D2" name="Range1"/>
   </protectedRanges>
@@ -8129,7 +8128,7 @@
   <dimension ref="A1:AR111"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8139,7 +8138,7 @@
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -8187,7 +8186,7 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -8235,7 +8234,7 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -8283,7 +8282,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -8331,7 +8330,7 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -8379,7 +8378,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -8427,7 +8426,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -8475,7 +8474,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -8523,7 +8522,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -8571,7 +8570,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -8619,7 +8618,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -8667,7 +8666,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -8715,7 +8714,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -8763,7 +8762,7 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -8811,7 +8810,7 @@
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -8859,7 +8858,7 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>